<commit_message>
gua uptake tpd scenarios
</commit_message>
<xml_diff>
--- a/GUA work/Pt(100)/IR chamber/plot_GUA area.xlsx
+++ b/GUA work/Pt(100)/IR chamber/plot_GUA area.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manolis\Desktop\PycharmProjects\IRAS\IRAS\GUA work\Pt(100)\IR chamber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9174CF0-9147-4345-9CC1-0883AAFE7DD9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39955D89-1242-460E-B592-81812B2045AA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10172" tabRatio="500" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'uptake area'!$E$52,'uptake area'!$F$52</definedName>
-    <definedName name="solver_adj" localSheetId="5" hidden="1">'vert + sloped intg uptk'!$F$35</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'vert + sloped intg uptk'!$F$32</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'verti intg uptk'!$I$49</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
@@ -64,7 +64,7 @@
     <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'uptake area'!$C$64</definedName>
-    <definedName name="solver_opt" localSheetId="5" hidden="1">'vert + sloped intg uptk'!$I$33</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'vert + sloped intg uptk'!$H$32</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">'verti intg uptk'!$J$49</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="123">
   <si>
     <t>L</t>
   </si>
@@ -474,6 +474,15 @@
   <si>
     <t>Case 2b</t>
   </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>ML at 0.025L using CO</t>
+  </si>
+  <si>
+    <t>θgua</t>
+  </si>
 </sst>
 </file>
 
@@ -701,7 +710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -806,9 +815,15 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -3421,6 +3436,144 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:v>CO+f*GUA_2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="80000"/>
+                  <a:lumOff val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="80000"/>
+                    <a:lumOff val="20000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'verti intg uptk'!$A$17:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'verti intg uptk'!$K$17:$K$28</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>414593.55904093076</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500059.93120113597</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>673152.23144687654</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>708620.54534737347</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>962563.44504935667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1174739.6922637075</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1476666.8670730223</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1600000.6115143611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2127212.9691302609</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3494819.727596554</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6503298.6309170518</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-CF31-4414-B9AB-D33561E8F639}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="13"/>
           <c:order val="13"/>
           <c:tx>
@@ -3865,7 +4018,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$I$1</c15:sqref>
@@ -3906,7 +4059,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$2:$C$13</c15:sqref>
@@ -3957,7 +4110,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$I$2:$I$13</c15:sqref>
@@ -4007,7 +4160,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
@@ -4020,7 +4173,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$J$1</c15:sqref>
@@ -4067,7 +4220,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$2:$C$13</c15:sqref>
@@ -4118,7 +4271,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$J$2:$J$13</c15:sqref>
@@ -4168,7 +4321,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
@@ -4181,7 +4334,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$K$1</c15:sqref>
@@ -4228,7 +4381,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$2:$C$13</c15:sqref>
@@ -4279,7 +4432,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$K$2:$K$13</c15:sqref>
@@ -4329,7 +4482,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
@@ -4342,7 +4495,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$L$1</c15:sqref>
@@ -4389,7 +4542,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$2:$C$13</c15:sqref>
@@ -4440,7 +4593,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$L$2:$L$13</c15:sqref>
@@ -4490,7 +4643,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
@@ -4588,7 +4741,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$3:$A$5</c15:sqref>
@@ -4612,7 +4765,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$O$3:$O$5</c15:sqref>
@@ -4635,7 +4788,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
@@ -4681,7 +4834,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$17:$A$28</c15:sqref>
@@ -4732,7 +4885,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$G$17:$G$28</c15:sqref>
@@ -4782,159 +4935,9 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-CF31-4414-B9AB-D33561E8F639}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="12"/>
-                <c:order val="12"/>
-                <c:tx>
-                  <c:v>CO+f*GUA_2</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="80000"/>
-                        <a:lumOff val="20000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1">
-                          <a:lumMod val="80000"/>
-                          <a:lumOff val="20000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'verti intg uptk'!$A$17:$A$28</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1.5E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2.5000000000000001E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>5.0000000000000001E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>7.4999999999999997E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.01</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1.4999999999999999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2.5000000000000001E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>3.5000000000000003E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0.05</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0.09</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.15</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'verti intg uptk'!$K$17:$K$28</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>414593.55904093076</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>500059.93120113597</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>673152.23144687654</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>708620.54534737347</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>962563.44504935667</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1174739.6922637075</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>1476666.8670730223</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>1600000.6115143611</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>2127212.9691302609</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>3494819.727596554</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>6503298.6309170518</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{0000000D-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -4981,7 +4984,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$17:$A$28</c15:sqref>
@@ -5032,7 +5035,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$G$17:$G$28</c15:sqref>
@@ -5082,7 +5085,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-CF31-4414-B9AB-D33561E8F639}"/>
                   </c:ext>
@@ -6483,7 +6486,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$H$1</c15:sqref>
@@ -6524,7 +6527,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$2:$C$13</c15:sqref>
@@ -6575,7 +6578,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$H$2:$H$13</c15:sqref>
@@ -6625,7 +6628,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-D62A-4FA1-BCD7-CBF8127C26B8}"/>
                   </c:ext>
@@ -6638,7 +6641,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$I$1</c15:sqref>
@@ -6679,7 +6682,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$A$2:$C$13</c15:sqref>
@@ -6730,7 +6733,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'verti intg uptk'!$I$2:$I$13</c15:sqref>
@@ -6780,7 +6783,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-D62A-4FA1-BCD7-CBF8127C26B8}"/>
                   </c:ext>
@@ -7802,167 +7805,12 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="5"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'vert + sloped intg uptk'!$I$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>GUA second + recom</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="19050" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$13</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1.5E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>2.5000000000000001E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>5.0000000000000001E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>7.4999999999999997E-3</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.01</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>1.4999999999999999E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>2.5000000000000001E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>3.5000000000000003E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>0.05</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>0.09</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>0.15</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>'vert + sloped intg uptk'!$I$2:$I$13</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>#,##0</c:formatCode>
-                      <c:ptCount val="12"/>
-                      <c:pt idx="0">
-                        <c:v>-1.4210854715202004E-14</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>331.12153575149</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>990.74102956659692</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1676.9380370154699</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1767.6644527446642</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>3212.4570288802947</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>4345.1299578032622</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>5235.7569750857438</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>5777.345741592203</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>5866.8134412203117</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>6167.6063970395126</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>5723.8335915159323</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000005-B95E-4EF6-88AA-01DC0792ED20}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
                 <c:idx val="0"/>
                 <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$B$1</c15:sqref>
                         </c15:formulaRef>
@@ -8003,7 +7851,7 @@
                 <c:xVal>
                   <c:numRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$13</c15:sqref>
                         </c15:formulaRef>
@@ -8054,7 +7902,7 @@
                 <c:yVal>
                   <c:numRef>
                     <c:extLst>
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$B$2:$B$13</c15:sqref>
                         </c15:formulaRef>
@@ -8116,7 +7964,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$D$1</c15:sqref>
@@ -8157,7 +8005,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$13</c15:sqref>
@@ -8208,7 +8056,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$E$2:$E$13</c15:sqref>
@@ -8258,7 +8106,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -8271,7 +8119,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$G$1</c15:sqref>
@@ -8312,7 +8160,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$13</c15:sqref>
@@ -8363,7 +8211,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$G$2:$G$13</c15:sqref>
@@ -8413,7 +8261,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -8426,7 +8274,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$H$1</c15:sqref>
@@ -8467,7 +8315,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$13</c15:sqref>
@@ -8518,7 +8366,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$H$2:$H$13</c15:sqref>
@@ -8568,9 +8416,164 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-B95E-4EF6-88AA-01DC0792ED20}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'vert + sloped intg uptk'!$I$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>GUA second + recom</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.5E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>2.5000000000000001E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.0000000000000001E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>7.4999999999999997E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.01</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1.4999999999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2.5000000000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.5000000000000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.05</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.09</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.15</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'vert + sloped intg uptk'!$I$2:$I$13</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>#,##0</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>-1.4210854715202004E-14</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>331.12153575149</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>990.74102956659692</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>1676.9380370154699</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>1767.6644527446642</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>3212.4570288802947</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>4345.1299578032622</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>5235.7569750857438</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>5777.345741592203</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>5866.8134412203117</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6167.6063970395126</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>5723.8335915159323</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -8667,7 +8670,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$2:$A$4</c15:sqref>
@@ -8691,7 +8694,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$C$2:$C$4</c15:sqref>
@@ -8714,7 +8717,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -8812,7 +8815,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$3:$A$5</c15:sqref>
@@ -8836,7 +8839,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$C$3:$C$5</c15:sqref>
@@ -8859,7 +8862,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -8872,7 +8875,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$C$18</c15:sqref>
@@ -8919,7 +8922,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -8970,7 +8973,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$C$19:$C$30</c15:sqref>
@@ -9020,7 +9023,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -9033,7 +9036,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$K$17</c15:sqref>
@@ -9083,7 +9086,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -9134,7 +9137,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$K$19:$K$30</c15:sqref>
@@ -9184,7 +9187,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -9197,7 +9200,7 @@
                 <c:order val="14"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$L$17</c15:sqref>
@@ -9247,7 +9250,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -9298,7 +9301,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$L$19:$L$30</c15:sqref>
@@ -9348,7 +9351,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -9361,7 +9364,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$M$17</c15:sqref>
@@ -9411,7 +9414,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -9462,7 +9465,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$M$19:$M$30</c15:sqref>
@@ -9512,7 +9515,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000011-B95E-4EF6-88AA-01DC0792ED20}"/>
                   </c:ext>
@@ -9526,6 +9529,7 @@
         <c:axId val="881002656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -9643,6 +9647,7 @@
         <c:axId val="868150512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -10972,7 +10977,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11127,7 +11132,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11282,7 +11287,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11437,7 +11442,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11583,7 +11588,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000E-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11728,7 +11733,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11889,7 +11894,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000011-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -11902,7 +11907,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$J$17</c15:sqref>
@@ -11952,7 +11957,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -12003,7 +12008,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$J$19:$J$30</c15:sqref>
@@ -12053,7 +12058,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -12066,7 +12071,7 @@
                 <c:order val="14"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$L$17</c15:sqref>
@@ -12116,7 +12121,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -12167,7 +12172,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$L$19:$L$30</c15:sqref>
@@ -12217,7 +12222,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -12230,7 +12235,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$M$17</c15:sqref>
@@ -12280,7 +12285,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -12331,7 +12336,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$M$19:$M$30</c15:sqref>
@@ -12381,7 +12386,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-E73E-49B3-858A-C3E9FCC0F7E9}"/>
                   </c:ext>
@@ -12395,6 +12400,7 @@
         <c:axId val="881002656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -12512,6 +12518,7 @@
         <c:axId val="868150512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="6000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -13849,7 +13856,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14004,7 +14011,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14159,7 +14166,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14314,7 +14321,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14460,7 +14467,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000E-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14605,7 +14612,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14618,7 +14625,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$B$18</c15:sqref>
@@ -14665,7 +14672,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -14716,7 +14723,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$B$19:$B$30</c15:sqref>
@@ -14766,7 +14773,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14779,7 +14786,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$J$17</c15:sqref>
@@ -14829,7 +14836,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -14880,7 +14887,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$J$19:$J$30</c15:sqref>
@@ -14930,7 +14937,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -14943,7 +14950,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$K$17</c15:sqref>
@@ -14993,7 +15000,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -15044,7 +15051,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$K$19:$K$30</c15:sqref>
@@ -15094,7 +15101,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -15107,7 +15114,7 @@
                 <c:order val="15"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$M$17</c15:sqref>
@@ -15157,7 +15164,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -15208,7 +15215,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$M$19:$M$30</c15:sqref>
@@ -15258,7 +15265,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-54C6-4D6F-91A0-B3C2A37E302A}"/>
                   </c:ext>
@@ -15272,6 +15279,7 @@
         <c:axId val="881002656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -15389,6 +15397,8 @@
         <c:axId val="868150512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1500000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -16726,7 +16736,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -16881,7 +16891,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17036,7 +17046,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17191,7 +17201,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000C-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17337,7 +17347,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000E-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17482,7 +17492,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000010-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17495,7 +17505,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$B$18</c15:sqref>
@@ -17542,7 +17552,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -17593,7 +17603,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$B$19:$B$30</c15:sqref>
@@ -17643,7 +17653,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17656,7 +17666,7 @@
                 <c:order val="12"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$J$17</c15:sqref>
@@ -17706,7 +17716,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -17757,7 +17767,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$J$19:$J$30</c15:sqref>
@@ -17807,7 +17817,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17820,7 +17830,7 @@
                 <c:order val="13"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$K$17</c15:sqref>
@@ -17870,7 +17880,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -17921,7 +17931,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$K$19:$K$30</c15:sqref>
@@ -17971,7 +17981,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -17984,7 +17994,7 @@
                 <c:order val="14"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$L$17</c15:sqref>
@@ -18034,7 +18044,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$A$19:$A$30</c15:sqref>
@@ -18085,7 +18095,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'vert + sloped intg uptk'!$L$19:$L$30</c15:sqref>
@@ -18135,7 +18145,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-B1D9-43B6-AE65-3133EA9121F5}"/>
                   </c:ext>
@@ -18149,6 +18159,7 @@
         <c:axId val="881002656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -18266,6 +18277,8 @@
         <c:axId val="868150512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1500000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -38938,16 +38951,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>209261</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>20242</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>799465</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>178184</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>415638</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>121438</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>448890</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>88187</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -38974,16 +38987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>515388</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>153784</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66501</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>128846</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>332508</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>66502</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>357447</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>41563</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39016,15 +39029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>432262</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>124693</xdr:rowOff>
+      <xdr:colOff>390698</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133005</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>124690</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>74813</xdr:rowOff>
+      <xdr:colOff>83126</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>83126</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39052,15 +39065,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>133002</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>133005</xdr:rowOff>
+      <xdr:colOff>415635</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>58191</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1213655</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>83125</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>199503</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>8312</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -43621,8 +43634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4D5658-95D9-452B-9C87-7CE505A65620}">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView topLeftCell="G22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -43718,7 +43731,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="9">
-        <f t="shared" ref="K2:M2" si="0">D2-D$2</f>
+        <f t="shared" ref="K2:L2" si="0">D2-D$2</f>
         <v>0</v>
       </c>
       <c r="L2" s="9">
@@ -43734,7 +43747,7 @@
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>(H2/$Q$18)*$Q$19</f>
+        <f t="shared" ref="Q2:Q13" si="1">(H2/$Q$18)*$Q$19</f>
         <v>0</v>
       </c>
     </row>
@@ -43767,27 +43780,27 @@
         <v>61.702380744041022</v>
       </c>
       <c r="J3" s="9">
-        <f t="shared" ref="J3:J13" si="1">C3-C$2</f>
+        <f t="shared" ref="J3:J13" si="2">C3-C$2</f>
         <v>88.443560702123989</v>
       </c>
       <c r="K3" s="9">
-        <f t="shared" ref="K3:K13" si="2">D3-D$2</f>
+        <f t="shared" ref="K3:K13" si="3">D3-D$2</f>
         <v>936.81877980730917</v>
       </c>
       <c r="L3" s="9">
-        <f t="shared" ref="L3:L13" si="3">E3-E$2</f>
+        <f t="shared" ref="L3:L13" si="4">E3-E$2</f>
         <v>664.39019843134042</v>
       </c>
       <c r="M3" s="9">
-        <f t="shared" ref="M3:M13" si="4">F3-F$2</f>
+        <f t="shared" ref="M3:M13" si="5">F3-F$2</f>
         <v>1726.7175341507595</v>
       </c>
       <c r="O3" s="7">
-        <f t="shared" ref="O3:O13" si="5">M3+H3</f>
+        <f t="shared" ref="O3:O13" si="6">M3+H3</f>
         <v>371219.42262163665</v>
       </c>
       <c r="Q3">
-        <f>(H3/$Q$18)*$Q$19</f>
+        <f t="shared" si="1"/>
         <v>0.12625603209564973</v>
       </c>
     </row>
@@ -43820,27 +43833,27 @@
         <v>153.49410905686699</v>
       </c>
       <c r="J4" s="9">
+        <f t="shared" si="2"/>
+        <v>99.319682212585292</v>
+      </c>
+      <c r="K4" s="9">
+        <f t="shared" si="3"/>
+        <v>1318.520198774685</v>
+      </c>
+      <c r="L4" s="9">
+        <f t="shared" si="4"/>
+        <v>1505.9448113947897</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" si="5"/>
+        <v>2979.5296505011347</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" si="6"/>
+        <v>425215.88579695905</v>
+      </c>
+      <c r="Q4">
         <f t="shared" si="1"/>
-        <v>99.319682212585292</v>
-      </c>
-      <c r="K4" s="9">
-        <f t="shared" si="2"/>
-        <v>1318.520198774685</v>
-      </c>
-      <c r="L4" s="9">
-        <f t="shared" si="3"/>
-        <v>1505.9448113947897</v>
-      </c>
-      <c r="M4" s="9">
-        <f t="shared" si="4"/>
-        <v>2979.5296505011347</v>
-      </c>
-      <c r="O4" s="7">
-        <f t="shared" si="5"/>
-        <v>425215.88579695905</v>
-      </c>
-      <c r="Q4">
-        <f>(H4/$Q$18)*$Q$19</f>
         <v>0.14427859115907318</v>
       </c>
     </row>
@@ -43873,27 +43886,27 @@
         <v>229.73054905644801</v>
       </c>
       <c r="J5" s="9">
+        <f t="shared" si="2"/>
+        <v>515.38094202489287</v>
+      </c>
+      <c r="K5" s="9">
+        <f t="shared" si="3"/>
+        <v>1913.2837889054858</v>
+      </c>
+      <c r="L5" s="9">
+        <f t="shared" si="4"/>
+        <v>3187.328306859984</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="5"/>
+        <v>5801.0000325729079</v>
+      </c>
+      <c r="O5" s="7">
+        <f t="shared" si="6"/>
+        <v>527434.49718821782</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="1"/>
-        <v>515.38094202489287</v>
-      </c>
-      <c r="K5" s="9">
-        <f t="shared" si="2"/>
-        <v>1913.2837889054858</v>
-      </c>
-      <c r="L5" s="9">
-        <f t="shared" si="3"/>
-        <v>3187.328306859984</v>
-      </c>
-      <c r="M5" s="9">
-        <f t="shared" si="4"/>
-        <v>5801.0000325729079</v>
-      </c>
-      <c r="O5" s="7">
-        <f t="shared" si="5"/>
-        <v>527434.49718821782</v>
-      </c>
-      <c r="Q5">
-        <f>(H5/$Q$18)*$Q$19</f>
         <v>0.17824269505795895</v>
       </c>
     </row>
@@ -43926,27 +43939,27 @@
         <v>342.87304976849401</v>
       </c>
       <c r="J6" s="9">
+        <f t="shared" si="2"/>
+        <v>778.7480986484486</v>
+      </c>
+      <c r="K6" s="9">
+        <f t="shared" si="3"/>
+        <v>1999.3409708528811</v>
+      </c>
+      <c r="L6" s="9">
+        <f t="shared" si="4"/>
+        <v>3555.3050576372711</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="5"/>
+        <v>6538.1319505742376</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="6"/>
+        <v>544386.48763797118</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="1"/>
-        <v>778.7480986484486</v>
-      </c>
-      <c r="K6" s="9">
-        <f t="shared" si="2"/>
-        <v>1999.3409708528811</v>
-      </c>
-      <c r="L6" s="9">
-        <f t="shared" si="3"/>
-        <v>3555.3050576372711</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="shared" si="4"/>
-        <v>6538.1319505742376</v>
-      </c>
-      <c r="O6" s="7">
-        <f t="shared" si="5"/>
-        <v>544386.48763797118</v>
-      </c>
-      <c r="Q6">
-        <f>(H6/$Q$18)*$Q$19</f>
         <v>0.18378332866458613</v>
       </c>
     </row>
@@ -43979,27 +43992,27 @@
         <v>547.75542111203504</v>
       </c>
       <c r="J7" s="9">
+        <f t="shared" si="2"/>
+        <v>3612.9412114549659</v>
+      </c>
+      <c r="K7" s="9">
+        <f t="shared" si="3"/>
+        <v>3193.0074205254159</v>
+      </c>
+      <c r="L7" s="9">
+        <f t="shared" si="4"/>
+        <v>7233.8487221567721</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" si="5"/>
+        <v>14532.764857944363</v>
+      </c>
+      <c r="O7" s="7">
+        <f t="shared" si="6"/>
+        <v>597508.87588496727</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="1"/>
-        <v>3612.9412114549659</v>
-      </c>
-      <c r="K7" s="9">
-        <f t="shared" si="2"/>
-        <v>3193.0074205254159</v>
-      </c>
-      <c r="L7" s="9">
-        <f t="shared" si="3"/>
-        <v>7233.8487221567721</v>
-      </c>
-      <c r="M7" s="9">
-        <f t="shared" si="4"/>
-        <v>14532.764857944363</v>
-      </c>
-      <c r="O7" s="7">
-        <f t="shared" si="5"/>
-        <v>597508.87588496727</v>
-      </c>
-      <c r="Q7">
-        <f>(H7/$Q$18)*$Q$19</f>
         <v>0.19920352843609554</v>
       </c>
     </row>
@@ -44032,27 +44045,27 @@
         <v>696.85043635950103</v>
       </c>
       <c r="J8" s="9">
+        <f t="shared" si="2"/>
+        <v>5596.7653614826413</v>
+      </c>
+      <c r="K8" s="9">
+        <f t="shared" si="3"/>
+        <v>4951.1614391790408</v>
+      </c>
+      <c r="L8" s="9">
+        <f t="shared" si="4"/>
+        <v>9970.4491196380895</v>
+      </c>
+      <c r="M8" s="9">
+        <f t="shared" si="5"/>
+        <v>21201.078990986742</v>
+      </c>
+      <c r="O8" s="7">
+        <f t="shared" si="6"/>
+        <v>642180.96496523265</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="1"/>
-        <v>5596.7653614826413</v>
-      </c>
-      <c r="K8" s="9">
-        <f t="shared" si="2"/>
-        <v>4951.1614391790408</v>
-      </c>
-      <c r="L8" s="9">
-        <f t="shared" si="3"/>
-        <v>9970.4491196380895</v>
-      </c>
-      <c r="M8" s="9">
-        <f t="shared" si="4"/>
-        <v>21201.078990986742</v>
-      </c>
-      <c r="O8" s="7">
-        <f t="shared" si="5"/>
-        <v>642180.96496523265</v>
-      </c>
-      <c r="Q8">
-        <f>(H8/$Q$18)*$Q$19</f>
         <v>0.21218945688184485</v>
       </c>
     </row>
@@ -44085,27 +44098,27 @@
         <v>909.93309697389407</v>
       </c>
       <c r="J9" s="9">
+        <f t="shared" si="2"/>
+        <v>11200.618764440449</v>
+      </c>
+      <c r="K9" s="9">
+        <f t="shared" si="3"/>
+        <v>6324.6245208367454</v>
+      </c>
+      <c r="L9" s="9">
+        <f t="shared" si="4"/>
+        <v>14268.560136117139</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" si="5"/>
+        <v>32784.837376983247</v>
+      </c>
+      <c r="O9" s="7">
+        <f t="shared" si="6"/>
+        <v>653130.8915881702</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="1"/>
-        <v>11200.618764440449</v>
-      </c>
-      <c r="K9" s="9">
-        <f t="shared" si="2"/>
-        <v>6324.6245208367454</v>
-      </c>
-      <c r="L9" s="9">
-        <f t="shared" si="3"/>
-        <v>14268.560136117139</v>
-      </c>
-      <c r="M9" s="9">
-        <f t="shared" si="4"/>
-        <v>32784.837376983247</v>
-      </c>
-      <c r="O9" s="7">
-        <f t="shared" si="5"/>
-        <v>653130.8915881702</v>
-      </c>
-      <c r="Q9">
-        <f>(H9/$Q$18)*$Q$19</f>
         <v>0.21197287592552777</v>
       </c>
     </row>
@@ -44150,15 +44163,15 @@
         <v>16155.30408450072</v>
       </c>
       <c r="M10" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>37549.209539675998</v>
       </c>
       <c r="O10" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>656786.3886903699</v>
       </c>
       <c r="Q10">
-        <f>(H10/$Q$18)*$Q$19</f>
+        <f t="shared" si="1"/>
         <v>0.21159397219265294</v>
       </c>
     </row>
@@ -44191,15 +44204,15 @@
         <v>1020.0124737153441</v>
       </c>
       <c r="J11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23988.480803216229</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10525.039312210896</v>
       </c>
       <c r="L11" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>21507.070842327761</v>
       </c>
       <c r="M11" s="9">
@@ -44207,11 +44220,11 @@
         <v>57878.526064943158</v>
       </c>
       <c r="O11" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>673338.18322139815</v>
       </c>
       <c r="Q11">
-        <f>(H11/$Q$18)*$Q$19</f>
+        <f t="shared" si="1"/>
         <v>0.21030318909577497</v>
       </c>
     </row>
@@ -44244,27 +44257,27 @@
         <v>1071.3432244094338</v>
       </c>
       <c r="J12" s="9">
+        <f t="shared" si="2"/>
+        <v>56027.682921549196</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="3"/>
+        <v>15875.794708432246</v>
+      </c>
+      <c r="L12" s="9">
+        <f t="shared" si="4"/>
+        <v>35002.597935338294</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="5"/>
+        <v>110133.35496122229</v>
+      </c>
+      <c r="O12" s="7">
+        <f t="shared" si="6"/>
+        <v>728334.1456035442</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="1"/>
-        <v>56027.682921549196</v>
-      </c>
-      <c r="K12" s="9">
-        <f t="shared" si="2"/>
-        <v>15875.794708432246</v>
-      </c>
-      <c r="L12" s="9">
-        <f t="shared" si="3"/>
-        <v>35002.597935338294</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" si="4"/>
-        <v>110133.35496122229</v>
-      </c>
-      <c r="O12" s="7">
-        <f t="shared" si="5"/>
-        <v>728334.1456035442</v>
-      </c>
-      <c r="Q12">
-        <f>(H12/$Q$18)*$Q$19</f>
         <v>0.21123983718815917</v>
       </c>
     </row>
@@ -44297,27 +44310,27 @@
         <v>1021.8198180778239</v>
       </c>
       <c r="J13" s="9">
+        <f t="shared" si="2"/>
+        <v>124221.42678498491</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="3"/>
+        <v>29699.793993883948</v>
+      </c>
+      <c r="L13" s="9">
+        <f t="shared" si="4"/>
+        <v>62843.873201213864</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" si="5"/>
+        <v>225142.8614983017</v>
+      </c>
+      <c r="O13" s="7">
+        <f t="shared" si="6"/>
+        <v>847841.38598878763</v>
+      </c>
+      <c r="Q13">
         <f t="shared" si="1"/>
-        <v>124221.42678498491</v>
-      </c>
-      <c r="K13" s="9">
-        <f t="shared" si="2"/>
-        <v>29699.793993883948</v>
-      </c>
-      <c r="L13" s="9">
-        <f t="shared" si="3"/>
-        <v>62843.873201213864</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" si="4"/>
-        <v>225142.8614983017</v>
-      </c>
-      <c r="O13" s="7">
-        <f t="shared" si="5"/>
-        <v>847841.38598878763</v>
-      </c>
-      <c r="Q13">
-        <f>(H13/$Q$18)*$Q$19</f>
         <v>0.21277671740601634</v>
       </c>
     </row>
@@ -44392,11 +44405,11 @@
         <v>1.5E-3</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" ref="G18:G28" si="6">A18*$G$15+$H$15</f>
+        <f t="shared" ref="G18:G28" si="7">A18*$G$15+$H$15</f>
         <v>369552</v>
       </c>
       <c r="H18" s="8">
-        <f t="shared" ref="H18:H28" si="7">G18-O3</f>
+        <f t="shared" ref="H18:H28" si="8">G18-O3</f>
         <v>-1667.4226216366515</v>
       </c>
       <c r="I18">
@@ -44404,11 +44417,11 @@
         <v>-0.96566032872118213</v>
       </c>
       <c r="J18">
-        <f t="shared" ref="J18:J28" si="8">(G18-(H3+$I$31*M3))^2</f>
+        <f t="shared" ref="J18:J28" si="9">(G18-(H3+$I$31*M3))^2</f>
         <v>2028742040.8376517</v>
       </c>
       <c r="K18" s="7">
-        <f t="shared" ref="K18:K28" si="9">H3+$I$31*M3</f>
+        <f t="shared" ref="K18:K28" si="10">H3+$I$31*M3</f>
         <v>414593.55904093076</v>
       </c>
       <c r="P18" t="s">
@@ -44423,23 +44436,23 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>409552</v>
       </c>
       <c r="H19" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-15663.885796959046</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I28" si="10">H19/(M4)</f>
+        <f t="shared" ref="I19:I28" si="11">H19/(M4)</f>
         <v>-5.2571672828711398</v>
       </c>
       <c r="J19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>8191685610.3095627</v>
       </c>
       <c r="K19" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>500059.93120113597</v>
       </c>
       <c r="P19" t="s">
@@ -44454,15 +44467,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G20" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>509552</v>
       </c>
       <c r="H20" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-17882.497188217822</v>
       </c>
       <c r="I20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-3.0826576603700566</v>
       </c>
       <c r="J20">
@@ -44470,7 +44483,7 @@
         <v>26765035729.471573</v>
       </c>
       <c r="K20" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>673152.23144687654</v>
       </c>
     </row>
@@ -44479,23 +44492,23 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="G21" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>609552</v>
       </c>
       <c r="H21" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>65165.512362028821</v>
       </c>
       <c r="I21">
+        <f t="shared" si="11"/>
+        <v>9.9669925377240816</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="9"/>
+        <v>9814576677.2445927</v>
+      </c>
+      <c r="K21" s="7">
         <f t="shared" si="10"/>
-        <v>9.9669925377240816</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="8"/>
-        <v>9814576677.2445927</v>
-      </c>
-      <c r="K21" s="7">
-        <f t="shared" si="9"/>
         <v>708620.54534737347</v>
       </c>
     </row>
@@ -44504,23 +44517,23 @@
         <v>0.01</v>
       </c>
       <c r="G22" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>709552</v>
       </c>
       <c r="H22" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>112043.12411503273</v>
       </c>
       <c r="I22">
+        <f t="shared" si="11"/>
+        <v>7.7096908406788227</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>64014791325.963631</v>
+      </c>
+      <c r="K22" s="7">
         <f t="shared" si="10"/>
-        <v>7.7096908406788227</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="8"/>
-        <v>64014791325.963631</v>
-      </c>
-      <c r="K22" s="7">
-        <f t="shared" si="9"/>
         <v>962563.44504935667</v>
       </c>
     </row>
@@ -44529,23 +44542,23 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G23" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>909552</v>
       </c>
       <c r="H23" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>267371.03503476735</v>
       </c>
       <c r="I23">
+        <f t="shared" si="11"/>
+        <v>12.611199418125622</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="9"/>
+        <v>70324512128.150833</v>
+      </c>
+      <c r="K23" s="7">
         <f t="shared" si="10"/>
-        <v>12.611199418125622</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="8"/>
-        <v>70324512128.150833</v>
-      </c>
-      <c r="K23" s="7">
-        <f t="shared" si="9"/>
         <v>1174739.6922637075</v>
       </c>
     </row>
@@ -44554,23 +44567,23 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G24" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1309552</v>
       </c>
       <c r="H24" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>656421.1084118298</v>
       </c>
       <c r="I24">
+        <f t="shared" si="11"/>
+        <v>20.022094386616462</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="9"/>
+        <v>27927378796.833912</v>
+      </c>
+      <c r="K24" s="7">
         <f t="shared" si="10"/>
-        <v>20.022094386616462</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="8"/>
-        <v>27927378796.833912</v>
-      </c>
-      <c r="K24" s="7">
-        <f t="shared" si="9"/>
         <v>1476666.8670730223</v>
       </c>
     </row>
@@ -44579,23 +44592,23 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G25" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1709552.0000000002</v>
       </c>
       <c r="H25" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1052765.6113096303</v>
       </c>
       <c r="I25">
+        <f t="shared" si="11"/>
+        <v>28.036958013649688</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="9"/>
+        <v>12001506719.131424</v>
+      </c>
+      <c r="K25" s="7">
         <f t="shared" si="10"/>
-        <v>28.036958013649688</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="8"/>
-        <v>12001506719.131424</v>
-      </c>
-      <c r="K25" s="7">
-        <f t="shared" si="9"/>
         <v>1600000.6115143611</v>
       </c>
       <c r="V25" t="s">
@@ -44610,23 +44623,23 @@
         <v>0.05</v>
       </c>
       <c r="G26" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2309552</v>
       </c>
       <c r="H26" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1636213.8167786018</v>
       </c>
       <c r="I26">
+        <f t="shared" si="11"/>
+        <v>28.269790680962959</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="9"/>
+        <v>33247522178.515678</v>
+      </c>
+      <c r="K26" s="7">
         <f t="shared" si="10"/>
-        <v>28.269790680962959</v>
-      </c>
-      <c r="J26">
-        <f t="shared" si="8"/>
-        <v>33247522178.515678</v>
-      </c>
-      <c r="K26" s="7">
-        <f t="shared" si="9"/>
         <v>2127212.9691302609</v>
       </c>
       <c r="U26">
@@ -44638,23 +44651,23 @@
         <v>0.09</v>
       </c>
       <c r="G27" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3909552</v>
       </c>
       <c r="H27" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3181217.8543964559</v>
       </c>
       <c r="I27">
+        <f t="shared" si="11"/>
+        <v>28.885144337213333</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="9"/>
+        <v>172002857772.92615</v>
+      </c>
+      <c r="K27" s="7">
         <f t="shared" si="10"/>
-        <v>28.885144337213333</v>
-      </c>
-      <c r="J27">
-        <f t="shared" si="8"/>
-        <v>172002857772.92615</v>
-      </c>
-      <c r="K27" s="7">
-        <f t="shared" si="9"/>
         <v>3494819.727596554</v>
       </c>
       <c r="V27" t="s">
@@ -44669,23 +44682,23 @@
         <v>0.15</v>
       </c>
       <c r="G28" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6309552</v>
       </c>
       <c r="H28" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5461710.6140112123</v>
       </c>
       <c r="I28">
+        <f t="shared" si="11"/>
+        <v>24.258866471111325</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="9"/>
+        <v>37537756991.708298</v>
+      </c>
+      <c r="K28" s="7">
         <f t="shared" si="10"/>
-        <v>24.258866471111325</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="8"/>
-        <v>37537756991.708298</v>
-      </c>
-      <c r="K28" s="7">
-        <f t="shared" si="9"/>
         <v>6503298.6309170518</v>
       </c>
     </row>
@@ -44791,11 +44804,11 @@
         <v>1.5E-3</v>
       </c>
       <c r="G36" s="8">
-        <f t="shared" ref="G36:G46" si="11">A36*$G$33</f>
+        <f t="shared" ref="G36:G46" si="12">A36*$G$33</f>
         <v>300000</v>
       </c>
       <c r="H36" s="8">
-        <f t="shared" ref="H36:H46" si="12">G36-O3</f>
+        <f t="shared" ref="H36:H46" si="13">G36-O3</f>
         <v>-71219.422621636651</v>
       </c>
       <c r="I36">
@@ -44803,11 +44816,11 @@
         <v>-41.245554766816014</v>
       </c>
       <c r="J36">
-        <f t="shared" ref="J36:J46" si="13">(G36-(H3+$I$49*M3))^2</f>
+        <f t="shared" ref="J36:J46" si="14">(G36-(H3+$I$49*M3))^2</f>
         <v>79172294166.790878</v>
       </c>
       <c r="K36" s="7">
-        <f t="shared" ref="K36:K46" si="14">H3+$I$49*M3</f>
+        <f t="shared" ref="K36:K46" si="15">H3+$I$49*M3</f>
         <v>581375.7170880083</v>
       </c>
     </row>
@@ -44816,19 +44829,19 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="G37" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>500000</v>
       </c>
       <c r="H37" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>74784.114203040954</v>
       </c>
       <c r="I37">
-        <f t="shared" ref="I37:I46" si="15">H37/(M4)</f>
+        <f t="shared" ref="I37:I46" si="16">H37/(M4)</f>
         <v>25.099301895003066</v>
       </c>
       <c r="J37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>82857698225.580658</v>
       </c>
       <c r="K37" s="7">
@@ -44841,15 +44854,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="G38" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1000000</v>
       </c>
       <c r="H38" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>472565.50281178218</v>
       </c>
       <c r="I38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>81.462765067799182</v>
       </c>
       <c r="J38">
@@ -44857,7 +44870,7 @@
         <v>54506290808.123222</v>
       </c>
       <c r="K38" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1233465.8236404704</v>
       </c>
     </row>
@@ -44866,23 +44879,23 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="G39" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1500000</v>
       </c>
       <c r="H39" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>955613.51236202882</v>
       </c>
       <c r="I39">
+        <f t="shared" si="16"/>
+        <v>146.16002240182661</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="14"/>
+        <v>25557434018.885662</v>
+      </c>
+      <c r="K39" s="7">
         <f t="shared" si="15"/>
-        <v>146.16002240182661</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="13"/>
-        <v>25557434018.885662</v>
-      </c>
-      <c r="K39" s="7">
-        <f t="shared" si="14"/>
         <v>1340133.0740306624</v>
       </c>
     </row>
@@ -44891,23 +44904,23 @@
         <v>0.01</v>
       </c>
       <c r="G40" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>2000000</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1402491.1241150326</v>
       </c>
       <c r="I40">
+        <f t="shared" si="16"/>
+        <v>96.505457689859909</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="14"/>
+        <v>134154206783.20578</v>
+      </c>
+      <c r="K40" s="7">
         <f t="shared" si="15"/>
-        <v>96.505457689859909</v>
-      </c>
-      <c r="J40">
-        <f t="shared" si="13"/>
-        <v>134154206783.20578</v>
-      </c>
-      <c r="K40" s="7">
-        <f t="shared" si="14"/>
         <v>2366270.6742058471</v>
       </c>
     </row>
@@ -44916,23 +44929,23 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="G41" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3000000</v>
       </c>
       <c r="H41" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2357819.0350347674</v>
       </c>
       <c r="I41">
+        <f t="shared" si="16"/>
+        <v>111.21221877608926</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="14"/>
+        <v>49521218652.920395</v>
+      </c>
+      <c r="K41" s="7">
         <f t="shared" si="15"/>
-        <v>111.21221877608926</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="13"/>
-        <v>49521218652.920395</v>
-      </c>
-      <c r="K41" s="7">
-        <f t="shared" si="14"/>
         <v>3222533.6348800343</v>
       </c>
     </row>
@@ -44941,23 +44954,23 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="G42" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5000000</v>
       </c>
       <c r="H42" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4346869.1084118299</v>
       </c>
       <c r="I42">
+        <f t="shared" si="16"/>
+        <v>132.58778924014339</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="14"/>
+        <v>127216309452.45322</v>
+      </c>
+      <c r="K42" s="7">
         <f t="shared" si="15"/>
-        <v>132.58778924014339</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="13"/>
-        <v>127216309452.45322</v>
-      </c>
-      <c r="K42" s="7">
-        <f t="shared" si="14"/>
         <v>4643326.0460133748</v>
       </c>
     </row>
@@ -44966,23 +44979,23 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="G43" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7000000.0000000009</v>
       </c>
       <c r="H43" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6343213.6113096308</v>
       </c>
       <c r="I43">
+        <f t="shared" si="16"/>
+        <v>168.93068293773635</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="14"/>
+        <v>3144073723388.3198</v>
+      </c>
+      <c r="K43" s="7">
         <f t="shared" si="15"/>
-        <v>168.93068293773635</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="13"/>
-        <v>3144073723388.3198</v>
-      </c>
-      <c r="K43" s="7">
-        <f t="shared" si="14"/>
         <v>5226846.3903574748</v>
       </c>
     </row>
@@ -44991,23 +45004,23 @@
         <v>0.05</v>
       </c>
       <c r="G44" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10000000</v>
       </c>
       <c r="H44" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9326661.8167786021</v>
       </c>
       <c r="I44">
+        <f t="shared" si="16"/>
+        <v>161.14200638616006</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="14"/>
+        <v>5209121953595.668</v>
+      </c>
+      <c r="K44" s="7">
         <f t="shared" si="15"/>
-        <v>161.14200638616006</v>
-      </c>
-      <c r="J44">
-        <f t="shared" si="13"/>
-        <v>5209121953595.668</v>
-      </c>
-      <c r="K44" s="7">
-        <f t="shared" si="14"/>
         <v>7717649.905558819</v>
       </c>
     </row>
@@ -45016,23 +45029,23 @@
         <v>0.09</v>
       </c>
       <c r="G45" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>18000000</v>
       </c>
       <c r="H45" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17271665.854396455</v>
       </c>
       <c r="I45">
+        <f t="shared" si="16"/>
+        <v>156.82502236019025</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="14"/>
+        <v>14957513405595.201</v>
+      </c>
+      <c r="K45" s="7">
         <f t="shared" si="15"/>
-        <v>156.82502236019025</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="13"/>
-        <v>14957513405595.201</v>
-      </c>
-      <c r="K45" s="7">
-        <f t="shared" si="14"/>
         <v>14132505.539034968</v>
       </c>
     </row>
@@ -45041,23 +45054,23 @@
         <v>0.15</v>
       </c>
       <c r="G46" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30000000</v>
       </c>
       <c r="H46" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29152158.614011213</v>
       </c>
       <c r="I46">
+        <f t="shared" si="16"/>
+        <v>129.48293550151539</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="14"/>
+        <v>3063712762062.7656</v>
+      </c>
+      <c r="K46" s="7">
         <f t="shared" si="15"/>
-        <v>129.48293550151539</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="13"/>
-        <v>3063712762062.7656</v>
-      </c>
-      <c r="K46" s="7">
-        <f t="shared" si="14"/>
         <v>28249653.530850887</v>
       </c>
     </row>
@@ -45092,10 +45105,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772DA03A-D901-4E93-9092-92428B426BE7}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -45189,11 +45202,11 @@
         <v>-1.4210854715202004E-14</v>
       </c>
       <c r="J2" s="7">
-        <f>SUM(E2,G2,H2)</f>
+        <f t="shared" ref="J2:J13" si="0">SUM(E2,G2,H2)</f>
         <v>0</v>
       </c>
       <c r="K2" s="7">
-        <f>C2+J2</f>
+        <f t="shared" ref="K2:K13" si="1">C2+J2</f>
         <v>0</v>
       </c>
     </row>
@@ -45231,11 +45244,11 @@
         <v>331.12153575149</v>
       </c>
       <c r="J3" s="7">
-        <f>SUM(E3,G3,H3)</f>
+        <f t="shared" si="0"/>
         <v>419.56509645361393</v>
       </c>
       <c r="K3" s="7">
-        <f>C3+J3</f>
+        <f t="shared" si="1"/>
         <v>369912.27018393949</v>
       </c>
     </row>
@@ -45273,11 +45286,11 @@
         <v>990.74102956659692</v>
       </c>
       <c r="J4" s="7">
-        <f>SUM(E4,G4,H4)</f>
+        <f t="shared" si="0"/>
         <v>1090.0607117791824</v>
       </c>
       <c r="K4" s="7">
-        <f>C4+J4</f>
+        <f t="shared" si="1"/>
         <v>423326.41685823706</v>
       </c>
     </row>
@@ -45315,11 +45328,11 @@
         <v>1676.9380370154699</v>
       </c>
       <c r="J5" s="7">
-        <f>SUM(E5,G5,H5)</f>
+        <f t="shared" si="0"/>
         <v>2192.318979040363</v>
       </c>
       <c r="K5" s="7">
-        <f>C5+J5</f>
+        <f t="shared" si="1"/>
         <v>523825.81613468524</v>
       </c>
     </row>
@@ -45357,11 +45370,11 @@
         <v>1767.6644527446642</v>
       </c>
       <c r="J6" s="7">
-        <f>SUM(E6,G6,H6)</f>
+        <f t="shared" si="0"/>
         <v>2546.4125513931126</v>
       </c>
       <c r="K6" s="7">
-        <f>C6+J6</f>
+        <f t="shared" si="1"/>
         <v>540394.7682387901</v>
       </c>
     </row>
@@ -45399,11 +45412,11 @@
         <v>3212.4570288802947</v>
       </c>
       <c r="J7" s="7">
-        <f>SUM(E7,G7,H7)</f>
+        <f t="shared" si="0"/>
         <v>6825.3982403352602</v>
       </c>
       <c r="K7" s="7">
-        <f>C7+J7</f>
+        <f t="shared" si="1"/>
         <v>589801.50926735823</v>
       </c>
     </row>
@@ -45441,11 +45454,11 @@
         <v>4345.1299578032622</v>
       </c>
       <c r="J8" s="7">
-        <f>SUM(E8,G8,H8)</f>
+        <f t="shared" si="0"/>
         <v>9941.8953192859026</v>
       </c>
       <c r="K8" s="7">
-        <f>C8+J8</f>
+        <f t="shared" si="1"/>
         <v>630921.78129353188</v>
       </c>
     </row>
@@ -45483,11 +45496,11 @@
         <v>5235.7569750857438</v>
       </c>
       <c r="J9" s="7">
-        <f>SUM(E9,G9,H9)</f>
+        <f t="shared" si="0"/>
         <v>16436.375739526193</v>
       </c>
       <c r="K9" s="7">
-        <f>C9+J9</f>
+        <f t="shared" si="1"/>
         <v>636782.42995071318</v>
       </c>
     </row>
@@ -45525,11 +45538,11 @@
         <v>5777.345741592203</v>
       </c>
       <c r="J10" s="7">
-        <f>SUM(E10,G10,H10)</f>
+        <f t="shared" si="0"/>
         <v>18424.113206563863</v>
       </c>
       <c r="K10" s="7">
-        <f>C10+J10</f>
+        <f t="shared" si="1"/>
         <v>637661.2923572578</v>
       </c>
     </row>
@@ -45567,11 +45580,11 @@
         <v>5866.8134412203117</v>
       </c>
       <c r="J11" s="7">
-        <f>SUM(E11,G11,H11)</f>
+        <f t="shared" si="0"/>
         <v>29855.29424443654</v>
       </c>
       <c r="K11" s="7">
-        <f>C11+J11</f>
+        <f t="shared" si="1"/>
         <v>645314.95140089153</v>
       </c>
     </row>
@@ -45609,11 +45622,11 @@
         <v>6167.6063970395126</v>
       </c>
       <c r="J12" s="7">
-        <f>SUM(E12,G12,H12)</f>
+        <f t="shared" si="0"/>
         <v>62195.289318588715</v>
       </c>
       <c r="K12" s="7">
-        <f>C12+J12</f>
+        <f t="shared" si="1"/>
         <v>680396.0799609106</v>
       </c>
     </row>
@@ -45651,11 +45664,11 @@
         <v>5723.8335915159323</v>
       </c>
       <c r="J13" s="7">
-        <f>SUM(E13,G13,H13)</f>
+        <f t="shared" si="0"/>
         <v>129945.26037650084</v>
       </c>
       <c r="K13" s="7">
-        <f>C13+J13</f>
+        <f t="shared" si="1"/>
         <v>752643.7848669868</v>
       </c>
     </row>
@@ -45756,19 +45769,19 @@
         <v>0</v>
       </c>
       <c r="B19" s="41">
-        <f>A19*$B$17</f>
+        <f t="shared" ref="B19:B30" si="2">A19*$B$17</f>
         <v>0</v>
       </c>
       <c r="C19" s="42">
-        <f>A19*$C$17+$C$16</f>
+        <f t="shared" ref="C19:C30" si="3">A19*$C$17+$C$16</f>
         <v>309521</v>
       </c>
       <c r="D19" s="42">
-        <f>B19-K2</f>
+        <f t="shared" ref="D19:D30" si="4">B19-K2</f>
         <v>0</v>
       </c>
       <c r="E19" s="42">
-        <f>C19-K2</f>
+        <f t="shared" ref="E19:E30" si="5">C19-K2</f>
         <v>309521</v>
       </c>
       <c r="F19" s="42">
@@ -45778,7 +45791,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="43">
-        <f>(B19-(C2+$F$33*J2))^2</f>
+        <f>(B19-(C2+$F$32*J2))^2</f>
         <v>0</v>
       </c>
       <c r="I19" s="44">
@@ -45807,19 +45820,19 @@
         <v>1.5E-3</v>
       </c>
       <c r="B20" s="45">
-        <f>A20*$B$17</f>
+        <f t="shared" si="2"/>
         <v>300000</v>
       </c>
       <c r="C20" s="46">
-        <f>A20*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>369521</v>
       </c>
       <c r="D20" s="46">
-        <f>B20-K3</f>
+        <f t="shared" si="4"/>
         <v>-69912.270183939487</v>
       </c>
       <c r="E20" s="46">
-        <f>C20-K3</f>
+        <f t="shared" si="5"/>
         <v>-391.27018393948674</v>
       </c>
       <c r="F20" s="46">
@@ -45831,27 +45844,27 @@
         <v>-0.93256132897304678</v>
       </c>
       <c r="H20" s="43">
-        <f t="shared" ref="H20:H30" si="0">(B20-(C3+$F$33*J3))^2</f>
-        <v>29129825465.984989</v>
+        <f t="shared" ref="H20:H30" si="6">(B20-(C3+$F$32*J3))^2</f>
+        <v>31029540985.676144</v>
       </c>
       <c r="I20" s="44">
-        <f t="shared" ref="I20:I30" si="1">(C20-(C3+$F$35*J3))^2</f>
+        <f t="shared" ref="I20:I29" si="7">(C20-(C3+$F$35*J3))^2</f>
         <v>370350242.04066366</v>
       </c>
       <c r="J20" s="9">
-        <f t="shared" ref="J20:J35" si="2">C3+$F$32*J3</f>
+        <f t="shared" ref="J20:J35" si="8">C3+$F$32*J3</f>
         <v>476152.03940254607</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" ref="K20:K30" si="3">C3+$F$33*J3</f>
+        <f t="shared" ref="K20:K30" si="9">C3+$F$33*J3</f>
         <v>470674.61869295326</v>
       </c>
       <c r="L20" s="9">
-        <f t="shared" ref="L20:L30" si="4">C3+$F$34*J3</f>
+        <f t="shared" ref="L20:L30" si="10">C3+$F$34*J3</f>
         <v>384386.88498789747</v>
       </c>
       <c r="M20" s="9">
-        <f t="shared" ref="M20:M30" si="5">C3+$F$35*J3</f>
+        <f t="shared" ref="M20:M30" si="11">C3+$F$35*J3</f>
         <v>388765.48601653636</v>
       </c>
     </row>
@@ -45860,51 +45873,51 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="B21" s="45">
-        <f>A21*$B$17</f>
+        <f t="shared" si="2"/>
         <v>500000</v>
       </c>
       <c r="C21" s="46">
-        <f>A21*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>409521</v>
       </c>
       <c r="D21" s="46">
-        <f>B21-K4</f>
+        <f t="shared" si="4"/>
         <v>76673.583141762938</v>
       </c>
       <c r="E21" s="46">
-        <f>C21-K4</f>
+        <f t="shared" si="5"/>
         <v>-13805.416858237062</v>
       </c>
       <c r="F21" s="46">
-        <f t="shared" ref="F21:F30" si="6">D21/J4</f>
+        <f t="shared" ref="F21:F30" si="12">D21/J4</f>
         <v>70.338819033865875</v>
       </c>
       <c r="G21" s="46">
-        <f t="shared" ref="G21:G30" si="7">E21/J4</f>
+        <f t="shared" ref="G21:G30" si="13">E21/J4</f>
         <v>-12.664814637437988</v>
       </c>
       <c r="H21" s="43">
-        <f t="shared" si="0"/>
-        <v>34267320738.092007</v>
+        <f t="shared" si="6"/>
+        <v>39738462278.696556</v>
       </c>
       <c r="I21" s="44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>3942263401.6756787</v>
       </c>
       <c r="J21" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>699345.08340738318</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>685114.3450359588</v>
       </c>
       <c r="L21" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>460932.52148728672</v>
       </c>
       <c r="M21" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>472308.44621081254</v>
       </c>
     </row>
@@ -45913,51 +45926,51 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B22" s="45">
-        <f>A22*$B$17</f>
+        <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
       <c r="C22" s="46">
-        <f>A22*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>509521</v>
       </c>
       <c r="D22" s="46">
-        <f>B22-K5</f>
+        <f t="shared" si="4"/>
         <v>476174.18386531476</v>
       </c>
       <c r="E22" s="46">
-        <f>C22-K5</f>
+        <f t="shared" si="5"/>
         <v>-14304.816134685243</v>
       </c>
       <c r="F22" s="46">
+        <f t="shared" si="12"/>
+        <v>217.20114108292262</v>
+      </c>
+      <c r="G22" s="46">
+        <f t="shared" si="13"/>
+        <v>-6.5249702581815194</v>
+      </c>
+      <c r="H22" s="43">
         <f t="shared" si="6"/>
-        <v>217.20114108292262</v>
-      </c>
-      <c r="G22" s="46">
+        <v>6233377473.4705591</v>
+      </c>
+      <c r="I22" s="44">
         <f t="shared" si="7"/>
-        <v>-6.5249702581815194</v>
-      </c>
-      <c r="H22" s="43">
-        <f t="shared" si="0"/>
-        <v>2533212141.8694215</v>
-      </c>
-      <c r="I22" s="44">
-        <f t="shared" si="1"/>
         <v>12727669552.138348</v>
       </c>
       <c r="J22" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1078951.7414213934</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1050331.0256389577</v>
       </c>
       <c r="L22" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>599458.82997982996</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>622337.97368808626</v>
       </c>
     </row>
@@ -45966,51 +45979,51 @@
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="B23" s="45">
-        <f>A23*$B$17</f>
+        <f t="shared" si="2"/>
         <v>1500000</v>
       </c>
       <c r="C23" s="46">
-        <f>A23*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>609521</v>
       </c>
       <c r="D23" s="46">
-        <f>B23-K6</f>
+        <f t="shared" si="4"/>
         <v>959605.2317612099</v>
       </c>
       <c r="E23" s="46">
-        <f>C23-K6</f>
+        <f t="shared" si="5"/>
         <v>69126.2317612099</v>
       </c>
       <c r="F23" s="46">
+        <f t="shared" si="12"/>
+        <v>376.8459400799847</v>
+      </c>
+      <c r="G23" s="46">
+        <f t="shared" si="13"/>
+        <v>27.146517057258354</v>
+      </c>
+      <c r="H23" s="43">
         <f t="shared" si="6"/>
-        <v>376.8459400799847</v>
-      </c>
-      <c r="G23" s="46">
+        <v>99110276015.425797</v>
+      </c>
+      <c r="I23" s="44">
         <f t="shared" si="7"/>
-        <v>27.146517057258354</v>
-      </c>
-      <c r="H23" s="43">
-        <f t="shared" si="0"/>
-        <v>121146634982.76881</v>
-      </c>
-      <c r="I23" s="44">
-        <f t="shared" si="1"/>
         <v>2051833574.1126113</v>
       </c>
       <c r="J23" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1185182.1542297422</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1151938.7482313367</v>
       </c>
       <c r="L23" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>628243.68876369868</v>
       </c>
       <c r="M23" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>654818.16960376897</v>
       </c>
     </row>
@@ -46019,51 +46032,51 @@
         <v>0.01</v>
       </c>
       <c r="B24" s="45">
-        <f>A24*$B$17</f>
+        <f t="shared" si="2"/>
         <v>2000000</v>
       </c>
       <c r="C24" s="46">
-        <f>A24*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>709521</v>
       </c>
       <c r="D24" s="46">
-        <f>B24-K7</f>
+        <f t="shared" si="4"/>
         <v>1410198.4907326419</v>
       </c>
       <c r="E24" s="46">
-        <f>C24-K7</f>
+        <f t="shared" si="5"/>
         <v>119719.49073264177</v>
       </c>
       <c r="F24" s="46">
+        <f t="shared" si="12"/>
+        <v>206.61043371783882</v>
+      </c>
+      <c r="G24" s="46">
+        <f t="shared" si="13"/>
+        <v>17.540293843244115</v>
+      </c>
+      <c r="H24" s="43">
         <f t="shared" si="6"/>
-        <v>206.61043371783882</v>
-      </c>
-      <c r="G24" s="46">
+        <v>101180045029.55783</v>
+      </c>
+      <c r="I24" s="44">
         <f t="shared" si="7"/>
-        <v>17.540293843244115</v>
-      </c>
-      <c r="H24" s="43">
-        <f t="shared" si="0"/>
-        <v>52433013384.375496</v>
-      </c>
-      <c r="I24" s="44">
-        <f t="shared" si="1"/>
         <v>34961792031.58284</v>
       </c>
       <c r="J24" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2318088.1089093992</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2228982.561310628</v>
       </c>
       <c r="L24" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>825271.55014428799</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>896501.72636392992</v>
       </c>
     </row>
@@ -46072,51 +46085,51 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="B25" s="45">
-        <f>A25*$B$17</f>
+        <f t="shared" si="2"/>
         <v>3000000</v>
       </c>
       <c r="C25" s="46">
-        <f>A25*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>909521</v>
       </c>
       <c r="D25" s="46">
-        <f>B25-K8</f>
+        <f t="shared" si="4"/>
         <v>2369078.2187064681</v>
       </c>
       <c r="E25" s="46">
-        <f>C25-K8</f>
+        <f t="shared" si="5"/>
         <v>278599.21870646812</v>
       </c>
       <c r="F25" s="46">
+        <f t="shared" si="12"/>
+        <v>238.29241232411528</v>
+      </c>
+      <c r="G25" s="46">
+        <f t="shared" si="13"/>
+        <v>28.022747148224759</v>
+      </c>
+      <c r="H25" s="43">
         <f t="shared" si="6"/>
-        <v>238.29241232411528</v>
-      </c>
-      <c r="G25" s="46">
+        <v>22007475644.885487</v>
+      </c>
+      <c r="I25" s="44">
         <f t="shared" si="7"/>
-        <v>28.022747148224759</v>
-      </c>
-      <c r="H25" s="43">
-        <f t="shared" si="0"/>
-        <v>344390571.21105129</v>
-      </c>
-      <c r="I25" s="44">
-        <f t="shared" si="1"/>
         <v>28271472254.749557</v>
       </c>
       <c r="J25" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3148349.1679952587</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3018557.7630982576</v>
       </c>
       <c r="L25" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>973908.14117975277</v>
       </c>
       <c r="M25" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1077662.2271120606</v>
       </c>
     </row>
@@ -46125,51 +46138,51 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="B26" s="45">
-        <f>A26*$B$17</f>
+        <f t="shared" si="2"/>
         <v>5000000</v>
       </c>
       <c r="C26" s="46">
-        <f>A26*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>1309521</v>
       </c>
       <c r="D26" s="46">
-        <f>B26-K9</f>
+        <f t="shared" si="4"/>
         <v>4363217.5700492868</v>
       </c>
       <c r="E26" s="46">
-        <f>C26-K9</f>
+        <f t="shared" si="5"/>
         <v>672738.57004928682</v>
       </c>
       <c r="F26" s="46">
+        <f t="shared" si="12"/>
+        <v>265.46105048916729</v>
+      </c>
+      <c r="G26" s="46">
+        <f t="shared" si="13"/>
+        <v>40.929860737576426</v>
+      </c>
+      <c r="H26" s="43">
         <f t="shared" si="6"/>
-        <v>265.46105048916729</v>
-      </c>
-      <c r="G26" s="46">
+        <v>40520328726.549553</v>
+      </c>
+      <c r="I26" s="44">
         <f t="shared" si="7"/>
-        <v>40.929860737576426</v>
-      </c>
-      <c r="H26" s="43">
-        <f t="shared" si="0"/>
-        <v>172950718431.46527</v>
-      </c>
-      <c r="I26" s="44">
-        <f t="shared" si="1"/>
         <v>4333885758.6303024</v>
       </c>
       <c r="J26" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4798703.3812341858</v>
       </c>
       <c r="K26" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4584126.5595983975</v>
       </c>
       <c r="L26" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1203822.4664401743</v>
       </c>
       <c r="M26" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1375353.2546980605</v>
       </c>
     </row>
@@ -46178,51 +46191,51 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="B27" s="45">
-        <f>A27*$B$17</f>
+        <f t="shared" si="2"/>
         <v>7000000.0000000009</v>
       </c>
       <c r="C27" s="46">
-        <f>A27*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>1709521.0000000002</v>
       </c>
       <c r="D27" s="46">
-        <f>B27-K10</f>
+        <f t="shared" si="4"/>
         <v>6362338.7076427434</v>
       </c>
       <c r="E27" s="46">
-        <f>C27-K10</f>
+        <f t="shared" si="5"/>
         <v>1071859.7076427424</v>
       </c>
       <c r="F27" s="46">
+        <f t="shared" si="12"/>
+        <v>345.32672679063143</v>
+      </c>
+      <c r="G27" s="46">
+        <f t="shared" si="13"/>
+        <v>58.177003996093369</v>
+      </c>
+      <c r="H27" s="43">
         <f t="shared" si="6"/>
-        <v>345.32672679063143</v>
-      </c>
-      <c r="G27" s="46">
+        <v>2880130557675.0469</v>
+      </c>
+      <c r="I27" s="44">
         <f t="shared" si="7"/>
-        <v>58.177003996093369</v>
-      </c>
-      <c r="H27" s="43">
-        <f t="shared" si="0"/>
-        <v>3754376949018.3662</v>
-      </c>
-      <c r="I27" s="44">
-        <f t="shared" si="1"/>
         <v>59521177421.921738</v>
       </c>
       <c r="J27" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5302905.2596643157</v>
       </c>
       <c r="K27" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5062378.5330931218</v>
       </c>
       <c r="L27" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1273276.4663163493</v>
       </c>
       <c r="M27" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1465551.3760261913</v>
       </c>
     </row>
@@ -46231,51 +46244,51 @@
         <v>0.05</v>
       </c>
       <c r="B28" s="45">
-        <f>A28*$B$17</f>
+        <f t="shared" si="2"/>
         <v>10000000</v>
       </c>
       <c r="C28" s="46">
-        <f>A28*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>2309521</v>
       </c>
       <c r="D28" s="46">
-        <f>B28-K11</f>
+        <f t="shared" si="4"/>
         <v>9354685.0485991091</v>
       </c>
       <c r="E28" s="46">
-        <f>C28-K11</f>
+        <f t="shared" si="5"/>
         <v>1664206.0485991086</v>
       </c>
       <c r="F28" s="46">
+        <f t="shared" si="12"/>
+        <v>313.33421040867256</v>
+      </c>
+      <c r="G28" s="46">
+        <f t="shared" si="13"/>
+        <v>55.742409871215031</v>
+      </c>
+      <c r="H28" s="43">
         <f t="shared" si="6"/>
-        <v>313.33421040867256</v>
-      </c>
-      <c r="G28" s="46">
+        <v>3221686310016.6226</v>
+      </c>
+      <c r="I28" s="44">
         <f t="shared" si="7"/>
-        <v>55.742409871215031</v>
-      </c>
-      <c r="H28" s="43">
-        <f t="shared" si="0"/>
-        <v>4772767304039.0576</v>
-      </c>
-      <c r="I28" s="44">
-        <f t="shared" si="1"/>
         <v>104105770642.6185</v>
       </c>
       <c r="J28" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8205094.3450931404</v>
       </c>
       <c r="K28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7815333.5943354974</v>
       </c>
       <c r="L28" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>1675295.4900580654</v>
       </c>
       <c r="M28" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1986866.7413226683</v>
       </c>
     </row>
@@ -46284,51 +46297,51 @@
         <v>0.09</v>
       </c>
       <c r="B29" s="45">
-        <f>A29*$B$17</f>
+        <f t="shared" si="2"/>
         <v>18000000</v>
       </c>
       <c r="C29" s="46">
-        <f>A29*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>3909521</v>
       </c>
       <c r="D29" s="46">
-        <f>B29-K12</f>
+        <f t="shared" si="4"/>
         <v>17319603.920039088</v>
       </c>
       <c r="E29" s="46">
-        <f>C29-K12</f>
+        <f t="shared" si="5"/>
         <v>3229124.9200390894</v>
       </c>
       <c r="F29" s="46">
+        <f t="shared" si="12"/>
+        <v>278.47131366044891</v>
+      </c>
+      <c r="G29" s="46">
+        <f t="shared" si="13"/>
+        <v>51.919123705627328</v>
+      </c>
+      <c r="H29" s="43">
         <f t="shared" si="6"/>
-        <v>278.47131366044891</v>
-      </c>
-      <c r="G29" s="46">
+        <v>2467676605710.5039</v>
+      </c>
+      <c r="I29" s="44">
         <f t="shared" si="7"/>
-        <v>51.919123705627328</v>
-      </c>
-      <c r="H29" s="43">
-        <f t="shared" si="0"/>
-        <v>5677942105037.2637</v>
-      </c>
-      <c r="I29" s="44">
-        <f t="shared" si="1"/>
         <v>188678134025.68134</v>
       </c>
       <c r="J29" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>16429115.979548298</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>15617156.71832215</v>
       </c>
       <c r="L29" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>2826077.0794451539</v>
       </c>
       <c r="M29" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>3475150.0363920704</v>
       </c>
     </row>
@@ -46337,32 +46350,32 @@
         <v>0.15</v>
       </c>
       <c r="B30" s="48">
-        <f>A30*$B$17</f>
+        <f t="shared" si="2"/>
         <v>30000000</v>
       </c>
       <c r="C30" s="49">
-        <f>A30*$C$17+$C$16</f>
+        <f t="shared" si="3"/>
         <v>6309521</v>
       </c>
       <c r="D30" s="49">
-        <f>B30-K13</f>
+        <f t="shared" si="4"/>
         <v>29247356.215133011</v>
       </c>
       <c r="E30" s="49">
-        <f>C30-K13</f>
+        <f t="shared" si="5"/>
         <v>5556877.2151330132</v>
       </c>
       <c r="F30" s="49">
+        <f t="shared" si="12"/>
+        <v>225.07443619253445</v>
+      </c>
+      <c r="G30" s="49">
+        <f t="shared" si="13"/>
+        <v>42.763215826669068</v>
+      </c>
+      <c r="H30" s="43">
         <f t="shared" si="6"/>
-        <v>225.07443619253445</v>
-      </c>
-      <c r="G30" s="49">
-        <f t="shared" si="7"/>
-        <v>42.763215826669068</v>
-      </c>
-      <c r="H30" s="43">
-        <f t="shared" si="0"/>
-        <v>3842274526449.1479</v>
+        <v>13370774288585.053</v>
       </c>
       <c r="I30" s="44">
         <f>(C30-(C13+$F$35*J13))^2</f>
@@ -46373,15 +46386,15 @@
         <v>33656606.936571807</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>31960172.065521073</v>
       </c>
       <c r="L30" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>5235637.2594155082</v>
       </c>
       <c r="M30" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6591752.0925143538</v>
       </c>
     </row>
@@ -46408,6 +46421,8 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="5" t="s">
         <v>107</v>
       </c>
@@ -46422,14 +46437,14 @@
       </c>
       <c r="H32">
         <f>SUM(H19:H26)</f>
-        <v>412805115715.76709</v>
+        <v>339819506154.26196</v>
       </c>
       <c r="I32">
         <f>SUM(I19:I26)</f>
         <v>182462516255.92999</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D33" s="5" t="s">
         <v>108</v>
       </c>
@@ -46444,39 +46459,85 @@
       </c>
       <c r="H33">
         <f>SUM(H19:H30)</f>
-        <v>18460166000259.602</v>
+        <v>22280087268141.488</v>
       </c>
       <c r="I33">
         <f>SUM(I19:I30)</f>
         <v>614421987927.99731</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D34" s="5" t="s">
         <v>109</v>
       </c>
       <c r="E34" s="58" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="60">
+      <c r="F34" s="59">
         <v>35.49909186036939</v>
       </c>
       <c r="I34" s="47"/>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D35" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E35" s="61" t="s">
+      <c r="E35" s="60" t="s">
         <v>101</v>
       </c>
       <c r="F35" s="62">
         <v>45.935138770965942</v>
       </c>
-      <c r="I35" s="47"/>
-      <c r="J35" t="e">
-        <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+      <c r="H35" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="I35" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="J35">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="H36" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="I36" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="J36" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="K36" s="55" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="G37" s="63" t="s">
+        <v>120</v>
+      </c>
+      <c r="H37" s="61">
+        <f>(B26/C9)*$J$35</f>
+        <v>0.60450130609251407</v>
+      </c>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61">
+        <f>(C26/C9)*J35</f>
+        <v>0.15832143097111501</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="G38" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="H38" s="61">
+        <f>(B26/C9)</f>
+        <v>8.0600174145668539</v>
+      </c>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61">
+        <f>(C26/C9)</f>
+        <v>2.1109524129482002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated gua ir fig
</commit_message>
<xml_diff>
--- a/GUA work/Pt(100)/IR chamber/plot_GUA area.xlsx
+++ b/GUA work/Pt(100)/IR chamber/plot_GUA area.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manolis\Desktop\PycharmProjects\IRAS\IRAS\GUA work\Pt(100)\IR chamber\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8B829B-5A2A-4E0C-9504-0DB069EF092A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17161766-54AE-4349-8705-F3F76148A4AE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14138" windowHeight="10172" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14138" windowHeight="10172" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="uptake old" sheetId="1" r:id="rId1"/>
@@ -50643,16 +50643,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>166253</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>54033</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>147781</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>192580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>290944</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>74814</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355598</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>19396</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -50835,16 +50835,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>650644</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>124365</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>226694</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>32924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>232756</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>307571</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>349134</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>24938</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -54920,8 +54920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -55563,7 +55563,7 @@
         <v>1041.8256310315001</v>
       </c>
       <c r="M13" s="3">
-        <f t="shared" si="5"/>
+        <f>((F13-$F$2)/$M$16)*$M$17</f>
         <v>0.79688102422343443</v>
       </c>
       <c r="N13" s="3">
@@ -55579,7 +55579,7 @@
         <v>6.1484910382375031E-2</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="3"/>
+        <f>((K13-$K$2)/$O$16)*$O$17</f>
         <v>1.2095047705168168E-2</v>
       </c>
       <c r="R13" s="3">
@@ -55627,7 +55627,11 @@
         <v>5834.2995908334397</v>
       </c>
     </row>
-    <row r="17" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f>K9/D9</f>
+        <v>2.615877781277973E-2</v>
+      </c>
       <c r="L17" t="s">
         <v>18</v>
       </c>
@@ -55641,7 +55645,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
       <c r="L19" t="s">
         <v>22</v>
       </c>
@@ -55652,7 +55656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M20">
         <v>0.1</v>
       </c>
@@ -55660,7 +55664,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="12:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
       <c r="M21">
         <v>0.2</v>
       </c>
@@ -57152,8 +57156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772DA03A-D901-4E93-9092-92428B426BE7}">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -57274,7 +57278,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="60">
-        <f t="shared" ref="M2:M7" si="1">E2/I2</f>
+        <f t="shared" ref="M2:M6" si="1">E2/I2</f>
         <v>0</v>
       </c>
       <c r="Q2" t="s">
@@ -58319,7 +58323,7 @@
         <v>2.2384332276334865E-2</v>
       </c>
       <c r="T22" s="3">
-        <f t="shared" ref="T21:T30" si="22">(($F$32*G5)/C5)*P22/2</f>
+        <f t="shared" ref="T22:T30" si="22">(($F$32*G5)/C5)*P22/2</f>
         <v>5.7014215339793679E-2</v>
       </c>
       <c r="U22" s="3">
@@ -58331,7 +58335,7 @@
         <v>3.1258049191410136E-3</v>
       </c>
       <c r="W22" s="3">
-        <f t="shared" ref="W21:W30" si="23">(($F$34*G5)/C5)*P22/2</f>
+        <f t="shared" ref="W22:W30" si="23">(($F$34*G5)/C5)*P22/2</f>
         <v>7.961609601306029E-3</v>
       </c>
       <c r="X22" s="3">
@@ -58588,7 +58592,7 @@
         <v>0.53789705199809645</v>
       </c>
       <c r="O25" s="3">
-        <f t="shared" si="18"/>
+        <f>(L25/C8)*(P25/2)</f>
         <v>0.1663926998259565</v>
       </c>
       <c r="P25" s="3">
@@ -59317,7 +59321,7 @@
         <v>119</v>
       </c>
       <c r="L36" s="60">
-        <f t="shared" ref="L36:L45" si="33">O20/$J$35</f>
+        <f t="shared" ref="L36:L44" si="33">O20/$J$35</f>
         <v>0.64384994350204128</v>
       </c>
       <c r="N36" s="3">

</xml_diff>